<commit_message>
use hv word; add link; read; dict btn
</commit_message>
<xml_diff>
--- a/test_universalApp/gui_design.xlsx
+++ b/test_universalApp/gui_design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10380" windowHeight="5865" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10380" windowHeight="5865"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>browser edit</t>
   </si>
@@ -274,6 +274,21 @@
   </si>
   <si>
     <t>paste</t>
+  </si>
+  <si>
+    <t>main page option</t>
+  </si>
+  <si>
+    <t>reading</t>
+  </si>
+  <si>
+    <t>kanji learning</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>dict size</t>
   </si>
 </sst>
 </file>
@@ -497,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -548,6 +563,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -820,7 +836,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -828,10 +844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,12 +855,12 @@
     <col min="1" max="24" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
         <v>31</v>
       </c>
@@ -857,7 +873,7 @@
       <c r="I2" s="22"/>
       <c r="J2" s="23"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -872,7 +888,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
         <v>1</v>
       </c>
@@ -897,7 +913,7 @@
       <c r="I4" s="25"/>
       <c r="J4" s="26"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B5" s="27"/>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
@@ -908,7 +924,7 @@
       <c r="I5" s="28"/>
       <c r="J5" s="29"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B6" s="27"/>
       <c r="C6" s="28"/>
       <c r="D6" s="28"/>
@@ -919,7 +935,7 @@
       <c r="I6" s="28"/>
       <c r="J6" s="29"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B7" s="27"/>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
@@ -930,7 +946,7 @@
       <c r="I7" s="28"/>
       <c r="J7" s="29"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B8" s="27"/>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
@@ -941,7 +957,7 @@
       <c r="I8" s="28"/>
       <c r="J8" s="29"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B9" s="27"/>
       <c r="C9" s="28"/>
       <c r="D9" s="28"/>
@@ -952,7 +968,7 @@
       <c r="I9" s="28"/>
       <c r="J9" s="29"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B10" s="27"/>
       <c r="C10" s="28"/>
       <c r="D10" s="28"/>
@@ -963,7 +979,7 @@
       <c r="I10" s="28"/>
       <c r="J10" s="29"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B11" s="27"/>
       <c r="C11" s="28"/>
       <c r="D11" s="28"/>
@@ -974,7 +990,7 @@
       <c r="I11" s="28"/>
       <c r="J11" s="29"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B12" s="27"/>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
@@ -984,8 +1000,11 @@
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
       <c r="J12" s="29"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B13" s="27"/>
       <c r="C13" s="28"/>
       <c r="D13" s="28"/>
@@ -995,8 +1014,18 @@
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
       <c r="J13" s="29"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S13" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="X13" s="3"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B14" s="27"/>
       <c r="C14" s="28"/>
       <c r="D14" s="28"/>
@@ -1006,8 +1035,16 @@
       <c r="H14" s="28"/>
       <c r="I14" s="28"/>
       <c r="J14" s="29"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="10"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B15" s="27"/>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
@@ -1017,8 +1054,14 @@
       <c r="H15" s="28"/>
       <c r="I15" s="28"/>
       <c r="J15" s="29"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S15" s="9"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="10"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B16" s="27"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
@@ -1028,8 +1071,16 @@
       <c r="H16" s="28"/>
       <c r="I16" s="28"/>
       <c r="J16" s="29"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S16" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="10"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B17" s="30"/>
       <c r="C17" s="31"/>
       <c r="D17" s="31"/>
@@ -1039,8 +1090,14 @@
       <c r="H17" s="31"/>
       <c r="I17" s="31"/>
       <c r="J17" s="32"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S17" s="1"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="2"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D18" s="18"/>
       <c r="F18" s="35" t="s">
         <v>8</v>
@@ -1053,8 +1110,14 @@
         <v>30</v>
       </c>
       <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="S18" s="11"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="45"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
@@ -1063,12 +1126,12 @@
       </c>
       <c r="J19" s="34"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B22" s="21" t="s">
         <v>17</v>
       </c>
@@ -1076,31 +1139,31 @@
       <c r="D22" s="22"/>
       <c r="E22" s="23"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
         <v>32</v>
       </c>
@@ -1412,7 +1475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V53"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T45" sqref="T45"/>
     </sheetView>
   </sheetViews>
@@ -2308,7 +2371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
rand, db file xml, speak search word
</commit_message>
<xml_diff>
--- a/test_universalApp/gui_design.xlsx
+++ b/test_universalApp/gui_design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10380" windowHeight="5865"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10380" windowHeight="5865" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="1">
+    <comment ref="D4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -103,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M11" authorId="1">
+    <comment ref="M4" authorId="1">
       <text>
         <r>
           <rPr>
@@ -116,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="1">
+    <comment ref="D5" authorId="1">
       <text>
         <r>
           <rPr>
@@ -129,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D14" authorId="1">
+    <comment ref="D7" authorId="1">
       <text>
         <r>
           <rPr>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>browser edit</t>
   </si>
@@ -216,24 +216,12 @@
     <t>Back</t>
   </si>
   <si>
-    <t>Next</t>
-  </si>
-  <si>
     <t>1/3</t>
   </si>
   <si>
     <t>Prev</t>
   </si>
   <si>
-    <t>Sulf</t>
-  </si>
-  <si>
-    <t>mark</t>
-  </si>
-  <si>
-    <t>edit</t>
-  </si>
-  <si>
     <t>next</t>
   </si>
   <si>
@@ -289,6 +277,24 @@
   </si>
   <si>
     <t>dict size</t>
+  </si>
+  <si>
+    <t>full dict</t>
+  </si>
+  <si>
+    <t>suft</t>
+  </si>
+  <si>
+    <t>setting</t>
+  </si>
+  <si>
+    <t>speak</t>
+  </si>
+  <si>
+    <t>star</t>
+  </si>
+  <si>
+    <t>&lt;extentd commands&gt;</t>
   </si>
 </sst>
 </file>
@@ -368,7 +374,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -508,11 +514,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -564,6 +583,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,7 +856,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -846,7 +866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
@@ -862,7 +882,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -1001,7 +1021,7 @@
       <c r="I12" s="28"/>
       <c r="J12" s="29"/>
       <c r="S12" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -1015,13 +1035,13 @@
       <c r="I13" s="28"/>
       <c r="J13" s="29"/>
       <c r="S13" s="46" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
       <c r="W13" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="X13" s="3"/>
     </row>
@@ -1036,7 +1056,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="29"/>
       <c r="S14" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
@@ -1072,7 +1092,7 @@
       <c r="I16" s="28"/>
       <c r="J16" s="29"/>
       <c r="S16" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
@@ -1103,11 +1123,11 @@
         <v>8</v>
       </c>
       <c r="G18" s="36" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="36" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J18" s="2"/>
       <c r="S18" s="11"/>
@@ -1122,7 +1142,7 @@
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
       <c r="I19" s="33" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J19" s="34"/>
     </row>
@@ -1165,10 +1185,10 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1182,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,7 +1222,7 @@
       </c>
       <c r="B2" s="8"/>
       <c r="D2" s="21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -1219,18 +1239,18 @@
         <v>12</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="D3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="2"/>
+      <c r="D3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="10"/>
       <c r="O3" s="18"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1238,18 +1258,20 @@
         <v>15</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="D4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="10"/>
+      <c r="D4" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="3"/>
       <c r="O4" s="18"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1257,7 +1279,9 @@
         <v>13</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="D5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -1270,7 +1294,9 @@
       <c r="O5" s="18"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -1283,20 +1309,24 @@
       <c r="O6" s="18"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D7" s="9"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="10"/>
+      <c r="D7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="45"/>
       <c r="O7" s="18"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -1304,7 +1334,6 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
       <c r="M8" s="10"/>
       <c r="O8" s="18"/>
     </row>
@@ -1317,44 +1346,38 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
       <c r="M9" s="10"/>
       <c r="O9" s="18"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D10" s="9"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="M10" s="45"/>
       <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D11" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="41" t="s">
+      <c r="D11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="3"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="2"/>
       <c r="O11" s="18"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D12" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="D12" s="9"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -1367,9 +1390,7 @@
       <c r="O12" s="18"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D13" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="D13" s="9"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -1381,25 +1402,18 @@
       <c r="M13" s="10"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="M14" s="20"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="M14" s="10"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D15" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="D15" s="9"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -1407,8 +1421,10 @@
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="19"/>
+      <c r="M15" s="10"/>
+      <c r="N15" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" s="9"/>
@@ -1419,50 +1435,62 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="M16" s="19"/>
-    </row>
-    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D17" s="11"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="20"/>
-    </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="F18" s="15" t="s">
+      <c r="M16" s="10"/>
+      <c r="N16" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="O16" s="19"/>
+    </row>
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D17" s="9"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="O17" s="20"/>
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D18" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="37"/>
+      <c r="G18" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="15"/>
+      <c r="I18" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="15"/>
+      <c r="K18" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="L18" s="37"/>
+      <c r="M18" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" s="37"/>
-      <c r="I18" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="J18" s="15"/>
-      <c r="K18" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="L18" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="M18" s="37"/>
-    </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D19" s="38" t="s">
         <v>21</v>
       </c>
       <c r="E19" s="37"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
+      <c r="L19" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="M19" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2386,11 +2414,11 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J3" s="2"/>
     </row>
@@ -2487,11 +2515,11 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J13" s="2"/>
     </row>
@@ -2503,7 +2531,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J14" s="45"/>
     </row>

</xml_diff>